<commit_message>
turned it into OOP
</commit_message>
<xml_diff>
--- a/Problem Data.xlsx
+++ b/Problem Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\PERSONAL PROJECTS\pioneersHackathon2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176AD5A4-E89B-4E80-948E-26CE32246216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD2C7E-1F17-48CF-9560-03858323D678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1AD1360B-DD42-40F0-810E-4A5C904D28E8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -573,35 +573,13 @@
   </si>
   <si>
     <t>One Silo or Transfer Station can be connected to maximum of 2 lines, except for Silo A and Silo B.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Raw</t>
-  </si>
-  <si>
-    <t>Blend</t>
-  </si>
-  <si>
-    <t>TCT</t>
-  </si>
-  <si>
-    <t>Blend Code Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -663,7 +641,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,30 +663,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,7 +731,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -805,13 +759,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -856,14 +803,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>754720</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>132047</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2647066" cy="569002"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -980,7 +927,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -1024,7 +971,6 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a:r>
                 <a:rPr lang="en-US" sz="1800" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -1059,8 +1005,8 @@
       <xdr:rowOff>190501</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>106087</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12060653</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>136071</xdr:rowOff>
     </xdr:to>
@@ -1429,10 +1375,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:O101"/>
+  <dimension ref="B2:O48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A64" zoomScale="76" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R76" sqref="R76"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="88" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1386,7 @@
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36" bestFit="1" customWidth="1"/>
@@ -1453,12 +1399,15 @@
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1483,370 +1432,538 @@
       <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="27" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="3">
         <v>30780</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="3">
         <v>1</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K4" s="5">
-        <f>SUM(G4,G25,G26,G32)</f>
-        <v>68326.559999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="22" t="s">
+      <c r="K4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N4" s="3">
+        <v>60000</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="3">
         <v>1302</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="3">
         <v>1</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="3">
-        <f>SUM(G24,G27)</f>
-        <v>20887</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="K5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="N5" s="3">
+        <v>20000</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="3">
         <v>233</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K6" s="5">
-        <f>SUM(G28,G31)</f>
-        <v>50505.216</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+      <c r="K6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="N6" s="3">
+        <v>50000</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="3">
         <v>3726</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="3">
         <v>2</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="3">
-        <f>SUM(G8,G9,G17,G18)</f>
-        <v>56477</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="K7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="N7" s="3">
+        <v>50000</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="3">
         <v>11328</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="K8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="N8" s="3">
+        <v>30000</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="3">
         <v>13680</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="3">
         <v>2</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="K9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="N9" s="3">
+        <v>45000</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="3">
         <v>28800</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="3">
         <v>3</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="K10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="N10" s="3">
+        <v>40000</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="3">
         <v>17820</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="3">
         <v>4</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="K11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="N11" s="3">
+        <v>15000</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="3">
         <v>3240</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="3">
         <v>5</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="K12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="3">
         <v>8640</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="3">
         <v>6</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="K13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N13" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="3">
         <v>8640</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="3">
         <v>7</v>
       </c>
       <c r="J14" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
+      <c r="K14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="N14" s="3">
+        <v>15000</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="3">
         <v>3240</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="3">
         <v>8</v>
       </c>
       <c r="J15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
+      <c r="K15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N15" s="3">
+        <v>2000</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="3">
         <v>12960</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
@@ -1869,7 +1986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
@@ -1891,8 +2008,11 @@
       <c r="H18" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
@@ -1914,8 +2034,20 @@
       <c r="H19" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1937,8 +2069,20 @@
       <c r="H20" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="3">
+        <v>6000</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>37</v>
       </c>
@@ -1960,8 +2104,20 @@
       <c r="H21" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="3">
+        <v>3000</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>37</v>
       </c>
@@ -1983,8 +2139,20 @@
       <c r="H22" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J22" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="3">
+        <v>800</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>37</v>
       </c>
@@ -2006,8 +2174,20 @@
       <c r="H23" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L23" s="3">
+        <v>3000</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2029,8 +2209,20 @@
       <c r="H24" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J24" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L24" s="3">
+        <v>4500</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
@@ -2052,8 +2244,20 @@
       <c r="H25" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J25" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L25" s="3">
+        <v>5000</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -2075,8 +2279,20 @@
       <c r="H26" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L26" s="3">
+        <v>4000</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
@@ -2098,8 +2314,20 @@
       <c r="H27" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J27" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>33</v>
       </c>
@@ -2121,8 +2349,20 @@
       <c r="H28" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J28" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
@@ -2144,8 +2384,20 @@
       <c r="H29" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J29" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>4</v>
       </c>
@@ -2167,8 +2419,20 @@
       <c r="H30" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J30" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>38</v>
       </c>
@@ -2191,10 +2455,22 @@
       <c r="H31" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L31" s="3">
+        <v>500</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>177</v>
+        <v>38</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>91</v>
@@ -2215,13 +2491,56 @@
       <c r="H32" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="J32" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L32" s="3">
+        <v>400</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J33" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L33" s="3">
+        <v>2500</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J34" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="3">
+        <v>600</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2231,23 +2550,22 @@
       <c r="D37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="6">
         <v>541.20000000000005</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="4">
         <v>0.8</v>
       </c>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="10"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>35</v>
       </c>
@@ -2257,9 +2575,9 @@
       <c r="D39" s="4">
         <v>0.71</v>
       </c>
-      <c r="E39" s="3"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>1</v>
       </c>
@@ -2269,9 +2587,9 @@
       <c r="D40" s="4">
         <v>0.71</v>
       </c>
-      <c r="E40" s="3"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>36</v>
       </c>
@@ -2281,9 +2599,9 @@
       <c r="D41" s="4">
         <v>0.83399999999999996</v>
       </c>
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
         <v>37</v>
       </c>
@@ -2293,9 +2611,14 @@
       <c r="D42" s="4">
         <v>0.85099999999999998</v>
       </c>
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>34</v>
       </c>
@@ -2305,9 +2628,14 @@
       <c r="D43" s="4">
         <v>0.83199999999999996</v>
       </c>
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="G43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>2</v>
       </c>
@@ -2317,9 +2645,14 @@
       <c r="D44" s="4">
         <v>0.8</v>
       </c>
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>33</v>
       </c>
@@ -2329,9 +2662,14 @@
       <c r="D45" s="4">
         <v>0.8</v>
       </c>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>5</v>
       </c>
@@ -2341,9 +2679,8 @@
       <c r="D46" s="4">
         <v>0.8</v>
       </c>
-      <c r="E46" s="3"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>4</v>
       </c>
@@ -2353,9 +2690,8 @@
       <c r="D47" s="4">
         <v>0.8</v>
       </c>
-      <c r="E47" s="3"/>
-    </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>38</v>
       </c>
@@ -2365,559 +2701,7 @@
       <c r="D48" s="4">
         <v>0.8</v>
       </c>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="54" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L54" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="56" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K56" s="25">
-        <f>D38*C38</f>
-        <v>432.96000000000004</v>
-      </c>
-      <c r="L56" s="10"/>
-      <c r="M56" s="9"/>
-      <c r="N56" s="9"/>
-    </row>
-    <row r="57" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L57" s="10"/>
-    </row>
-    <row r="58" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L58" s="10"/>
-    </row>
-    <row r="59" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L59" s="10"/>
-    </row>
-    <row r="60" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L60" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="M60" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L61" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="M61" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="62" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L62" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="M62" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L63" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="M63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="L66" s="10"/>
-    </row>
-    <row r="69" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J69" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J70" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K70" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M70" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="N70" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O70" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J71" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L71" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="M71" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="N71" s="3">
-        <v>60000</v>
-      </c>
-      <c r="O71" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J72" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L72" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="M72" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="N72" s="3">
-        <v>20000</v>
-      </c>
-      <c r="O72" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J73" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="M73" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="N73" s="3">
-        <v>50000</v>
-      </c>
-      <c r="O73" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J74" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="M74" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="N74" s="3">
-        <v>50000</v>
-      </c>
-      <c r="O74" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J75" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L75" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="M75" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="N75" s="3">
-        <v>30000</v>
-      </c>
-      <c r="O75" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J76" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K76" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L76" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="M76" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="N76" s="3">
-        <v>45000</v>
-      </c>
-      <c r="O76" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J77" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K77" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L77" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="M77" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="N77" s="3">
-        <v>40000</v>
-      </c>
-      <c r="O77" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J78" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K78" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L78" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="M78" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="N78" s="3">
-        <v>15000</v>
-      </c>
-      <c r="O78" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J79" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K79" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L79" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="M79" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="N79" s="3">
-        <v>0</v>
-      </c>
-      <c r="O79" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J80" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L80" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M80" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="N80" s="3">
-        <v>10000</v>
-      </c>
-      <c r="O80" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J81" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L81" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="M81" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="N81" s="3">
-        <v>15000</v>
-      </c>
-      <c r="O81" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J82" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="K82" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L82" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="M82" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="N82" s="3">
-        <v>2000</v>
-      </c>
-      <c r="O82" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J85" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="86" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J86" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K86" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M86" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="87" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J87" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="K87" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L87" s="3">
-        <v>6000</v>
-      </c>
-      <c r="M87" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="88" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J88" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="K88" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L88" s="3">
-        <v>3000</v>
-      </c>
-      <c r="M88" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="89" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J89" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L89" s="3">
-        <v>800</v>
-      </c>
-      <c r="M89" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J90" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K90" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L90" s="3">
-        <v>3000</v>
-      </c>
-      <c r="M90" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="91" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J91" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K91" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L91" s="3">
-        <v>4500</v>
-      </c>
-      <c r="M91" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="92" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J92" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K92" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L92" s="3">
-        <v>5000</v>
-      </c>
-      <c r="M92" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="93" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J93" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K93" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L93" s="3">
-        <v>4000</v>
-      </c>
-      <c r="M93" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="94" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J94" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="K94" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L94" s="3">
-        <v>0</v>
-      </c>
-      <c r="M94" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="95" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J95" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="K95" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L95" s="3">
-        <v>0</v>
-      </c>
-      <c r="M95" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="96" spans="10:15" x14ac:dyDescent="0.25">
-      <c r="J96" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K96" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L96" s="3">
-        <v>0</v>
-      </c>
-      <c r="M96" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="97" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J97" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K97" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L97" s="3">
-        <v>0</v>
-      </c>
-      <c r="M97" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="98" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J98" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K98" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L98" s="3">
-        <v>500</v>
-      </c>
-      <c r="M98" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J99" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K99" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L99" s="3">
-        <v>400</v>
-      </c>
-      <c r="M99" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="100" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J100" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="K100" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L100" s="3">
-        <v>2500</v>
-      </c>
-      <c r="M100" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="101" spans="10:13" x14ac:dyDescent="0.25">
-      <c r="J101" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="K101" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L101" s="3">
-        <v>600</v>
-      </c>
-      <c r="M101" s="3" t="s">
-        <v>127</v>
-      </c>
+      <c r="F48" s="10"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:H32">
@@ -2925,8 +2709,7 @@
     <sortCondition ref="H4:H32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2935,33 +2718,31 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:AE48"/>
+  <dimension ref="B2:AE22"/>
   <sheetViews>
-    <sheetView zoomScale="63" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:P9"/>
+    <sheetView zoomScale="69" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="204.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="20" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:31" ht="17.25" x14ac:dyDescent="0.4">
@@ -3807,10 +3588,10 @@
         <v>27</v>
       </c>
       <c r="W17" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="X17" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
@@ -3861,10 +3642,10 @@
         <v>27</v>
       </c>
       <c r="W18" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="X18" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
@@ -3882,22 +3663,6 @@
     <row r="22" spans="2:31" ht="17.25" x14ac:dyDescent="0.4">
       <c r="C22" s="16" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>179</v>
-      </c>
-      <c r="D48" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3988,7 +3753,7 @@
   <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>